<commit_message>
Fixed issue where leading zeroes were ignored in excel_read commands
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC76AE0-DFB7-4309-A351-BCFE4698DA24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13CCE4B-ECA2-4822-851E-5E0F52F29B61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>AssetID</t>
+  </si>
+  <si>
+    <t>00456789</t>
   </si>
 </sst>
 </file>
@@ -58,8 +61,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,52 +344,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>21534554</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>21354</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>121548</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>213454</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5313857</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>24357</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>1578465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated import functionality and creation of assets and employees
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13CCE4B-ECA2-4822-851E-5E0F52F29B61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FF5904-DA36-431B-988C-C13305C10AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39480" yWindow="1320" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>AssetID</t>
   </si>
   <si>
     <t>00456789</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>0000000</t>
+  </si>
+  <si>
+    <t>1111111</t>
+  </si>
+  <si>
+    <t>2222222</t>
   </si>
 </sst>
 </file>
@@ -344,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -355,48 +367,99 @@
     <col min="1" max="1" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>21534554</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>21354</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>121548</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>213454</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5313857</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>24357</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>1578465</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Basic Input format checking for search tab implemented
Check if the list of asset #'s entered is the same as the one that went thru regex. If it is the same, then nothing happens, else the user is notified of bad input and search looks for valid inputs only
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FF5904-DA36-431B-988C-C13305C10AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D22588C-AF3F-4ECD-9E4D-544FC08FD674}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39480" yWindow="1320" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="495" yWindow="1350" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,24 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>AssetID</t>
   </si>
   <si>
-    <t>00456789</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>0000000</t>
-  </si>
-  <si>
-    <t>1111111</t>
-  </si>
-  <si>
-    <t>2222222</t>
+    <t>E0000000</t>
+  </si>
+  <si>
+    <t>E1111111</t>
+  </si>
+  <si>
+    <t>E1212121</t>
+  </si>
+  <si>
+    <t>40000000</t>
+  </si>
+  <si>
+    <t>41111111</t>
+  </si>
+  <si>
+    <t>41212121</t>
+  </si>
+  <si>
+    <t>E6942000</t>
+  </si>
+  <si>
+    <t>43333333</t>
+  </si>
+  <si>
+    <t>E8787655</t>
+  </si>
+  <si>
+    <t>E3213214</t>
+  </si>
+  <si>
+    <t>49856473</t>
   </si>
 </sst>
 </file>
@@ -359,7 +380,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,52 +393,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>21534554</v>
-      </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>21354</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>121548</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>213454</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5313857</v>
+      <c r="A6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>24357</v>
+      <c r="A7" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -425,15 +446,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1578465</v>
+      <c r="A9" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -441,7 +462,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -449,7 +470,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -457,7 +478,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1</v>

</xml_diff>

<commit_message>
Import assets now imports RFID tags
Fixed excel layout format and now code allows RFID tags to be put into RFID Table.
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D22588C-AF3F-4ECD-9E4D-544FC08FD674}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6DFC70-154D-4300-913B-C1EA6954B77F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="1350" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3285" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,45 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>AssetID</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>E0000000</t>
-  </si>
-  <si>
-    <t>E1111111</t>
-  </si>
-  <si>
-    <t>E1212121</t>
-  </si>
-  <si>
-    <t>40000000</t>
-  </si>
-  <si>
-    <t>41111111</t>
-  </si>
-  <si>
-    <t>41212121</t>
-  </si>
-  <si>
-    <t>E6942000</t>
-  </si>
-  <si>
-    <t>43333333</t>
-  </si>
-  <si>
-    <t>E8787655</t>
-  </si>
-  <si>
-    <t>E3213214</t>
-  </si>
-  <si>
-    <t>49856473</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Asset ID</t>
+  </si>
+  <si>
+    <t>RFID Tag</t>
+  </si>
+  <si>
+    <t>4524534534werwerwerwer</t>
+  </si>
+  <si>
+    <t>waweaser</t>
+  </si>
+  <si>
+    <t>45245345345asrasrsar</t>
+  </si>
+  <si>
+    <t>45345345zxvzxvzxb</t>
+  </si>
+  <si>
+    <t>E1010101</t>
+  </si>
+  <si>
+    <t>E0101010</t>
+  </si>
+  <si>
+    <t>E6996696</t>
+  </si>
+  <si>
+    <t>4867530</t>
   </si>
 </sst>
 </file>
@@ -377,15 +368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E6:E7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,90 +390,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can now select .xlsx file from a file browser prompt - exception thrown if asset/employee is already in table
Not sure why exception is being thrown but it works for all new entries.  Need to troubleshoot tomorrow
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6DFC70-154D-4300-913B-C1EA6954B77F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD52F0AE-B0DC-44B3-9DC6-B165FD84DB72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3285" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Asset ID</t>
   </si>
@@ -28,38 +28,32 @@
     <t>RFID Tag</t>
   </si>
   <si>
-    <t>4524534534werwerwerwer</t>
-  </si>
-  <si>
     <t>waweaser</t>
   </si>
   <si>
-    <t>45245345345asrasrsar</t>
-  </si>
-  <si>
-    <t>45345345zxvzxvzxb</t>
-  </si>
-  <si>
-    <t>E1010101</t>
-  </si>
-  <si>
-    <t>E0101010</t>
-  </si>
-  <si>
-    <t>E6996696</t>
-  </si>
-  <si>
-    <t>4867530</t>
+    <t>e1264342</t>
+  </si>
+  <si>
+    <t>e1264343</t>
+  </si>
+  <si>
+    <t>e1264344</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,37 +384,30 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>45345</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="B3">
+        <v>45245345</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed exception being thrown
Import functions now allows user to select file to be imported, does not import existing asset or employee ID's.

File dialog should open in a specific directory like C:\, having trouble implementing this
</commit_message>
<xml_diff>
--- a/AssetList.xlsx
+++ b/AssetList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD52F0AE-B0DC-44B3-9DC6-B165FD84DB72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA1F9EE-2208-4F87-B0B9-730FFA7EDF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3285" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,16 +28,16 @@
     <t>RFID Tag</t>
   </si>
   <si>
-    <t>waweaser</t>
-  </si>
-  <si>
-    <t>e1264342</t>
-  </si>
-  <si>
-    <t>e1264343</t>
-  </si>
-  <si>
-    <t>e1264344</t>
+    <t>E0000000</t>
+  </si>
+  <si>
+    <t>E6394850</t>
+  </si>
+  <si>
+    <t>E2354657</t>
+  </si>
+  <si>
+    <t>m3m3tag</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +392,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>45245345</v>
@@ -400,10 +400,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>